<commit_message>
Add figures and test Dash
</commit_message>
<xml_diff>
--- a/Src/Results_insertion/output_insertion_high_[0, 1]_0.xlsx
+++ b/Src/Results_insertion/output_insertion_high_[0, 1]_0.xlsx
@@ -601,7 +601,7 @@
         <v>2</v>
       </c>
       <c r="O3" t="n">
-        <v>0</v>
+        <v>0.0005230903625488281</v>
       </c>
     </row>
     <row r="4">
@@ -742,7 +742,7 @@
         <v>4</v>
       </c>
       <c r="O6" t="n">
-        <v>0</v>
+        <v>0.0009996891021728516</v>
       </c>
     </row>
     <row r="7">
@@ -836,7 +836,7 @@
         <v>5</v>
       </c>
       <c r="O8" t="n">
-        <v>0.0009906291961669922</v>
+        <v>0.001005649566650391</v>
       </c>
     </row>
     <row r="9">
@@ -977,7 +977,7 @@
         <v>6</v>
       </c>
       <c r="O11" t="n">
-        <v>0.003673076629638672</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
@@ -1071,7 +1071,7 @@
         <v>7</v>
       </c>
       <c r="O13" t="n">
-        <v>0</v>
+        <v>0.001006603240966797</v>
       </c>
     </row>
     <row r="14">
@@ -1118,7 +1118,7 @@
         <v>7</v>
       </c>
       <c r="O14" t="n">
-        <v>0.1509816646575928</v>
+        <v>0.2026379108428955</v>
       </c>
     </row>
     <row r="15">
@@ -1165,7 +1165,7 @@
         <v>8</v>
       </c>
       <c r="O15" t="n">
-        <v>0.001135110855102539</v>
+        <v>0.001012563705444336</v>
       </c>
     </row>
     <row r="16">
@@ -1212,7 +1212,7 @@
         <v>9</v>
       </c>
       <c r="O16" t="n">
-        <v>0</v>
+        <v>0.001085758209228516</v>
       </c>
     </row>
     <row r="17">
@@ -1259,7 +1259,7 @@
         <v>10</v>
       </c>
       <c r="O17" t="n">
-        <v>0</v>
+        <v>0.001104116439819336</v>
       </c>
     </row>
     <row r="18">
@@ -1306,7 +1306,7 @@
         <v>11</v>
       </c>
       <c r="O18" t="n">
-        <v>0.001007556915283203</v>
+        <v>0.00201106071472168</v>
       </c>
     </row>
     <row r="19">
@@ -1353,7 +1353,7 @@
         <v>10</v>
       </c>
       <c r="O19" t="n">
-        <v>0</v>
+        <v>0.001000404357910156</v>
       </c>
     </row>
     <row r="20">
@@ -1400,7 +1400,7 @@
         <v>11</v>
       </c>
       <c r="O20" t="n">
-        <v>0</v>
+        <v>0.002087116241455078</v>
       </c>
     </row>
     <row r="21">
@@ -1447,7 +1447,7 @@
         <v>11</v>
       </c>
       <c r="O21" t="n">
-        <v>0.001421451568603516</v>
+        <v>0.0009996891021728516</v>
       </c>
     </row>
     <row r="22">
@@ -1541,7 +1541,7 @@
         <v>12</v>
       </c>
       <c r="O23" t="n">
-        <v>0.002002239227294922</v>
+        <v>0.001104593276977539</v>
       </c>
     </row>
     <row r="24">
@@ -1635,7 +1635,7 @@
         <v>14</v>
       </c>
       <c r="O25" t="n">
-        <v>0.09867262840270996</v>
+        <v>0.1101336479187012</v>
       </c>
     </row>
     <row r="26">
@@ -1682,7 +1682,7 @@
         <v>14</v>
       </c>
       <c r="O26" t="n">
-        <v>0.1131141185760498</v>
+        <v>0.1527211666107178</v>
       </c>
     </row>
     <row r="27">
@@ -1729,7 +1729,7 @@
         <v>15</v>
       </c>
       <c r="O27" t="n">
-        <v>0.01476883888244629</v>
+        <v>0.02155756950378418</v>
       </c>
     </row>
     <row r="28">
@@ -1776,7 +1776,7 @@
         <v>15</v>
       </c>
       <c r="O28" t="n">
-        <v>0</v>
+        <v>0.001002073287963867</v>
       </c>
     </row>
     <row r="29">
@@ -1823,7 +1823,7 @@
         <v>16</v>
       </c>
       <c r="O29" t="n">
-        <v>0.005072832107543945</v>
+        <v>0.009074687957763672</v>
       </c>
     </row>
     <row r="30">
@@ -1870,7 +1870,7 @@
         <v>16</v>
       </c>
       <c r="O30" t="n">
-        <v>0.007613420486450195</v>
+        <v>0.004054546356201172</v>
       </c>
     </row>
     <row r="31">
@@ -1917,7 +1917,7 @@
         <v>17</v>
       </c>
       <c r="O31" t="n">
-        <v>0.001863241195678711</v>
+        <v>0.001998662948608398</v>
       </c>
     </row>
     <row r="32">
@@ -2011,7 +2011,7 @@
         <v>19</v>
       </c>
       <c r="O33" t="n">
-        <v>0.002707481384277344</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34">
@@ -2058,7 +2058,7 @@
         <v>18</v>
       </c>
       <c r="O34" t="n">
-        <v>7.195422410964966</v>
+        <v>12.7786328792572</v>
       </c>
     </row>
     <row r="35">
@@ -2105,7 +2105,7 @@
         <v>19</v>
       </c>
       <c r="O35" t="n">
-        <v>0.01572132110595703</v>
+        <v>0.02059102058410645</v>
       </c>
     </row>
     <row r="36">
@@ -2152,7 +2152,7 @@
         <v>19</v>
       </c>
       <c r="O36" t="n">
-        <v>0.08480691909790039</v>
+        <v>0.1852035522460938</v>
       </c>
     </row>
     <row r="37">
@@ -2199,7 +2199,7 @@
         <v>21</v>
       </c>
       <c r="O37" t="n">
-        <v>0.1844727993011475</v>
+        <v>0.3207833766937256</v>
       </c>
     </row>
     <row r="38">
@@ -2246,7 +2246,7 @@
         <v>21</v>
       </c>
       <c r="O38" t="n">
-        <v>0</v>
+        <v>0.01584410667419434</v>
       </c>
     </row>
     <row r="39">
@@ -2293,7 +2293,7 @@
         <v>22</v>
       </c>
       <c r="O39" t="n">
-        <v>0</v>
+        <v>0.01582050323486328</v>
       </c>
     </row>
     <row r="40">
@@ -2340,7 +2340,7 @@
         <v>21</v>
       </c>
       <c r="O40" t="n">
-        <v>0.04958844184875488</v>
+        <v>0.1353545188903809</v>
       </c>
     </row>
     <row r="41">
@@ -2434,7 +2434,7 @@
         <v>20</v>
       </c>
       <c r="O42" t="n">
-        <v>0.06357765197753906</v>
+        <v>0.1510148048400879</v>
       </c>
     </row>
     <row r="43">
@@ -2481,7 +2481,7 @@
         <v>21</v>
       </c>
       <c r="O43" t="n">
-        <v>0.01000666618347168</v>
+        <v>0.003079414367675781</v>
       </c>
     </row>
     <row r="44">
@@ -2528,7 +2528,7 @@
         <v>21</v>
       </c>
       <c r="O44" t="n">
-        <v>0.06377744674682617</v>
+        <v>0.1099669933319092</v>
       </c>
     </row>
     <row r="45">
@@ -2622,7 +2622,7 @@
         <v>20</v>
       </c>
       <c r="O46" t="n">
-        <v>0</v>
+        <v>0.003000736236572266</v>
       </c>
     </row>
     <row r="47">
@@ -2669,7 +2669,7 @@
         <v>21</v>
       </c>
       <c r="O47" t="n">
-        <v>0</v>
+        <v>0.001042366027832031</v>
       </c>
     </row>
     <row r="48">
@@ -2716,7 +2716,7 @@
         <v>21</v>
       </c>
       <c r="O48" t="n">
-        <v>0.0679481029510498</v>
+        <v>0.1147842407226562</v>
       </c>
     </row>
     <row r="49">
@@ -2857,7 +2857,7 @@
         <v>16</v>
       </c>
       <c r="O51" t="n">
-        <v>0</v>
+        <v>0.007058143615722656</v>
       </c>
     </row>
     <row r="52">
@@ -2904,7 +2904,7 @@
         <v>17</v>
       </c>
       <c r="O52" t="n">
-        <v>0.002358913421630859</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53">
@@ -2998,7 +2998,7 @@
         <v>17</v>
       </c>
       <c r="O54" t="n">
-        <v>0</v>
+        <v>0.01011919975280762</v>
       </c>
     </row>
     <row r="55">
@@ -3045,7 +3045,7 @@
         <v>13</v>
       </c>
       <c r="O55" t="n">
-        <v>0.03148603439331055</v>
+        <v>0.06833338737487793</v>
       </c>
     </row>
     <row r="56">
@@ -3139,7 +3139,7 @@
         <v>10</v>
       </c>
       <c r="O57" t="n">
-        <v>0</v>
+        <v>0.0111076831817627</v>
       </c>
     </row>
     <row r="58">
@@ -3327,7 +3327,7 @@
         <v>12</v>
       </c>
       <c r="O61" t="n">
-        <v>0</v>
+        <v>0.001973152160644531</v>
       </c>
     </row>
     <row r="62">
@@ -3374,7 +3374,7 @@
         <v>12</v>
       </c>
       <c r="O62" t="n">
-        <v>0.02577304840087891</v>
+        <v>0.01300740242004395</v>
       </c>
     </row>
     <row r="63">
@@ -3421,7 +3421,7 @@
         <v>13</v>
       </c>
       <c r="O63" t="n">
-        <v>0</v>
+        <v>0.0006785392761230469</v>
       </c>
     </row>
     <row r="64">
@@ -3468,7 +3468,7 @@
         <v>14</v>
       </c>
       <c r="O64" t="n">
-        <v>0.0005509853363037109</v>
+        <v>0</v>
       </c>
     </row>
     <row r="65">
@@ -3515,7 +3515,7 @@
         <v>9</v>
       </c>
       <c r="O65" t="n">
-        <v>0.05144977569580078</v>
+        <v>0.09147787094116211</v>
       </c>
     </row>
     <row r="66">
@@ -3562,7 +3562,7 @@
         <v>9</v>
       </c>
       <c r="O66" t="n">
-        <v>0.005611658096313477</v>
+        <v>0.009242773056030273</v>
       </c>
     </row>
     <row r="67">
@@ -3656,7 +3656,7 @@
         <v>11</v>
       </c>
       <c r="O68" t="n">
-        <v>0.001004457473754883</v>
+        <v>0</v>
       </c>
     </row>
     <row r="69">
@@ -3703,7 +3703,7 @@
         <v>6</v>
       </c>
       <c r="O69" t="n">
-        <v>0.006958723068237305</v>
+        <v>0.01540732383728027</v>
       </c>
     </row>
     <row r="70">
@@ -3750,7 +3750,7 @@
         <v>6</v>
       </c>
       <c r="O70" t="n">
-        <v>0</v>
+        <v>0.001875638961791992</v>
       </c>
     </row>
     <row r="71">
@@ -3797,7 +3797,7 @@
         <v>9</v>
       </c>
       <c r="O71" t="n">
-        <v>0.01558446884155273</v>
+        <v>0.02425336837768555</v>
       </c>
     </row>
     <row r="72">
@@ -3844,7 +3844,7 @@
         <v>8</v>
       </c>
       <c r="O72" t="n">
-        <v>125.5066449642181</v>
+        <v>138.5756075382233</v>
       </c>
     </row>
     <row r="73">
@@ -3891,7 +3891,7 @@
         <v>7</v>
       </c>
       <c r="O73" t="n">
-        <v>0.01706886291503906</v>
+        <v>0.01060843467712402</v>
       </c>
     </row>
     <row r="74">
@@ -3985,7 +3985,7 @@
         <v>7</v>
       </c>
       <c r="O75" t="n">
-        <v>0.002474784851074219</v>
+        <v>0</v>
       </c>
     </row>
     <row r="76">
@@ -4032,7 +4032,7 @@
         <v>8</v>
       </c>
       <c r="O76" t="n">
-        <v>0.002002954483032227</v>
+        <v>0</v>
       </c>
     </row>
     <row r="77">
@@ -4079,7 +4079,7 @@
         <v>9</v>
       </c>
       <c r="O77" t="n">
-        <v>0</v>
+        <v>0.01604676246643066</v>
       </c>
     </row>
     <row r="78">
@@ -4267,7 +4267,7 @@
         <v>13</v>
       </c>
       <c r="O81" t="n">
-        <v>0.04996109008789062</v>
+        <v>0.05000948905944824</v>
       </c>
     </row>
     <row r="82">
@@ -4455,7 +4455,7 @@
         <v>17</v>
       </c>
       <c r="O85" t="n">
-        <v>0.001949071884155273</v>
+        <v>0</v>
       </c>
     </row>
     <row r="86">
@@ -4502,7 +4502,7 @@
         <v>18</v>
       </c>
       <c r="O86" t="n">
-        <v>0.0124976634979248</v>
+        <v>0</v>
       </c>
     </row>
     <row r="87">
@@ -4549,7 +4549,7 @@
         <v>19</v>
       </c>
       <c r="O87" t="n">
-        <v>0.009103059768676758</v>
+        <v>0.007982969284057617</v>
       </c>
     </row>
     <row r="88">
@@ -4690,7 +4690,7 @@
         <v>18</v>
       </c>
       <c r="O90" t="n">
-        <v>0.1586627960205078</v>
+        <v>0.1330914497375488</v>
       </c>
     </row>
     <row r="91">
@@ -4972,7 +4972,7 @@
         <v>21</v>
       </c>
       <c r="O96" t="n">
-        <v>0.1263649463653564</v>
+        <v>0.08298754692077637</v>
       </c>
     </row>
     <row r="97">
@@ -5019,7 +5019,7 @@
         <v>22</v>
       </c>
       <c r="O97" t="n">
-        <v>0.01591825485229492</v>
+        <v>0</v>
       </c>
     </row>
     <row r="98">
@@ -5066,7 +5066,7 @@
         <v>23</v>
       </c>
       <c r="O98" t="n">
-        <v>0</v>
+        <v>0.008511781692504883</v>
       </c>
     </row>
     <row r="99">
@@ -5160,7 +5160,7 @@
         <v>23</v>
       </c>
       <c r="O100" t="n">
-        <v>0.08257603645324707</v>
+        <v>0.07381963729858398</v>
       </c>
     </row>
     <row r="101">
@@ -5301,7 +5301,7 @@
         <v>21</v>
       </c>
       <c r="O103" t="n">
-        <v>0.03164315223693848</v>
+        <v>0.03437972068786621</v>
       </c>
     </row>
     <row r="104">
@@ -5348,7 +5348,7 @@
         <v>21</v>
       </c>
       <c r="O104" t="n">
-        <v>3.37287974357605</v>
+        <v>3.656021595001221</v>
       </c>
     </row>
     <row r="105">
@@ -5395,7 +5395,7 @@
         <v>19</v>
       </c>
       <c r="O105" t="n">
-        <v>0.03247475624084473</v>
+        <v>0.02335095405578613</v>
       </c>
     </row>
     <row r="106">
@@ -5442,7 +5442,7 @@
         <v>19</v>
       </c>
       <c r="O106" t="n">
-        <v>0.06367039680480957</v>
+        <v>0.04840922355651855</v>
       </c>
     </row>
     <row r="107">
@@ -5489,7 +5489,7 @@
         <v>19</v>
       </c>
       <c r="O107" t="n">
-        <v>0.03188323974609375</v>
+        <v>0.03774404525756836</v>
       </c>
     </row>
     <row r="108">
@@ -5536,7 +5536,7 @@
         <v>20</v>
       </c>
       <c r="O108" t="n">
-        <v>0.005606651306152344</v>
+        <v>0.01321983337402344</v>
       </c>
     </row>
     <row r="109">
@@ -5583,7 +5583,7 @@
         <v>17</v>
       </c>
       <c r="O109" t="n">
-        <v>0</v>
+        <v>0.01050257682800293</v>
       </c>
     </row>
     <row r="110">
@@ -5630,7 +5630,7 @@
         <v>17</v>
       </c>
       <c r="O110" t="n">
-        <v>0.05716300010681152</v>
+        <v>0.05618071556091309</v>
       </c>
     </row>
     <row r="111">
@@ -5677,7 +5677,7 @@
         <v>14</v>
       </c>
       <c r="O111" t="n">
-        <v>0.001000881195068359</v>
+        <v>0</v>
       </c>
     </row>
     <row r="112">
@@ -5724,7 +5724,7 @@
         <v>14</v>
       </c>
       <c r="O112" t="n">
-        <v>0.01657724380493164</v>
+        <v>0.02182388305664062</v>
       </c>
     </row>
     <row r="113">
@@ -5771,7 +5771,7 @@
         <v>14</v>
       </c>
       <c r="O113" t="n">
-        <v>0.01631975173950195</v>
+        <v>0.03330779075622559</v>
       </c>
     </row>
     <row r="114">
@@ -5818,7 +5818,7 @@
         <v>14</v>
       </c>
       <c r="O114" t="n">
-        <v>0.003748178482055664</v>
+        <v>0.01650452613830566</v>
       </c>
     </row>
     <row r="115">
@@ -5865,7 +5865,7 @@
         <v>14</v>
       </c>
       <c r="O115" t="n">
-        <v>0.01725864410400391</v>
+        <v>0.01251626014709473</v>
       </c>
     </row>
     <row r="116">
@@ -5912,7 +5912,7 @@
         <v>9</v>
       </c>
       <c r="O116" t="n">
-        <v>0.01639842987060547</v>
+        <v>0.0126183032989502</v>
       </c>
     </row>
     <row r="117">
@@ -5959,7 +5959,7 @@
         <v>9</v>
       </c>
       <c r="O117" t="n">
-        <v>0.01578712463378906</v>
+        <v>0.0210573673248291</v>
       </c>
     </row>
     <row r="118">
@@ -6006,7 +6006,7 @@
         <v>7</v>
       </c>
       <c r="O118" t="n">
-        <v>0.015472412109375</v>
+        <v>0</v>
       </c>
     </row>
     <row r="119">
@@ -6100,7 +6100,7 @@
         <v>8</v>
       </c>
       <c r="O120" t="n">
-        <v>0.0009992122650146484</v>
+        <v>0</v>
       </c>
     </row>
     <row r="121">
@@ -6147,7 +6147,7 @@
         <v>9</v>
       </c>
       <c r="O121" t="n">
-        <v>0.001001119613647461</v>
+        <v>0</v>
       </c>
     </row>
     <row r="122">
@@ -6194,7 +6194,7 @@
         <v>10</v>
       </c>
       <c r="O122" t="n">
-        <v>0.002019882202148438</v>
+        <v>0</v>
       </c>
     </row>
     <row r="123">
@@ -6382,7 +6382,7 @@
         <v>8</v>
       </c>
       <c r="O126" t="n">
-        <v>0.001186132431030273</v>
+        <v>0</v>
       </c>
     </row>
     <row r="127">
@@ -6523,7 +6523,7 @@
         <v>10</v>
       </c>
       <c r="O129" t="n">
-        <v>0.01565313339233398</v>
+        <v>0.001497268676757812</v>
       </c>
     </row>
     <row r="130">
@@ -6617,7 +6617,7 @@
         <v>8</v>
       </c>
       <c r="O131" t="n">
-        <v>0.001505613327026367</v>
+        <v>0.0003156661987304688</v>
       </c>
     </row>
     <row r="132">
@@ -6664,7 +6664,7 @@
         <v>9</v>
       </c>
       <c r="O132" t="n">
-        <v>0.009735107421875</v>
+        <v>0</v>
       </c>
     </row>
     <row r="133">
@@ -6711,7 +6711,7 @@
         <v>10</v>
       </c>
       <c r="O133" t="n">
-        <v>0.001004457473754883</v>
+        <v>0</v>
       </c>
     </row>
     <row r="134">
@@ -6758,7 +6758,7 @@
         <v>8</v>
       </c>
       <c r="O134" t="n">
-        <v>0.002414464950561523</v>
+        <v>0</v>
       </c>
     </row>
     <row r="135">
@@ -6805,7 +6805,7 @@
         <v>9</v>
       </c>
       <c r="O135" t="n">
-        <v>0.0009973049163818359</v>
+        <v>0.0005707740783691406</v>
       </c>
     </row>
     <row r="136">
@@ -6852,7 +6852,7 @@
         <v>10</v>
       </c>
       <c r="O136" t="n">
-        <v>0.001316070556640625</v>
+        <v>0.0009629726409912109</v>
       </c>
     </row>
     <row r="137">
@@ -6899,7 +6899,7 @@
         <v>7</v>
       </c>
       <c r="O137" t="n">
-        <v>0.001000404357910156</v>
+        <v>0</v>
       </c>
     </row>
     <row r="138">
@@ -6946,7 +6946,7 @@
         <v>8</v>
       </c>
       <c r="O138" t="n">
-        <v>0.002312660217285156</v>
+        <v>0.0009996891021728516</v>
       </c>
     </row>
     <row r="139">
@@ -6993,7 +6993,7 @@
         <v>8</v>
       </c>
       <c r="O139" t="n">
-        <v>0.001000165939331055</v>
+        <v>0</v>
       </c>
     </row>
     <row r="140">
@@ -7040,7 +7040,7 @@
         <v>8</v>
       </c>
       <c r="O140" t="n">
-        <v>0.003528118133544922</v>
+        <v>0</v>
       </c>
     </row>
     <row r="141">
@@ -7087,7 +7087,7 @@
         <v>9</v>
       </c>
       <c r="O141" t="n">
-        <v>0.001535892486572266</v>
+        <v>0</v>
       </c>
     </row>
     <row r="142">
@@ -7134,7 +7134,7 @@
         <v>9</v>
       </c>
       <c r="O142" t="n">
-        <v>0.00099945068359375</v>
+        <v>0.0161592960357666</v>
       </c>
     </row>
     <row r="143">
@@ -7181,7 +7181,7 @@
         <v>10</v>
       </c>
       <c r="O143" t="n">
-        <v>0.001021385192871094</v>
+        <v>0</v>
       </c>
     </row>
     <row r="144">
@@ -7228,7 +7228,7 @@
         <v>10</v>
       </c>
       <c r="O144" t="n">
-        <v>0.002001523971557617</v>
+        <v>0</v>
       </c>
     </row>
     <row r="145">
@@ -7275,7 +7275,7 @@
         <v>11</v>
       </c>
       <c r="O145" t="n">
-        <v>0.001065969467163086</v>
+        <v>0</v>
       </c>
     </row>
     <row r="146">
@@ -7322,7 +7322,7 @@
         <v>8</v>
       </c>
       <c r="O146" t="n">
-        <v>0</v>
+        <v>0.001001119613647461</v>
       </c>
     </row>
     <row r="147">
@@ -7416,7 +7416,7 @@
         <v>8</v>
       </c>
       <c r="O148" t="n">
-        <v>0.001753568649291992</v>
+        <v>0.01062870025634766</v>
       </c>
     </row>
     <row r="149">
@@ -7463,7 +7463,7 @@
         <v>8</v>
       </c>
       <c r="O149" t="n">
-        <v>0.001501321792602539</v>
+        <v>0</v>
       </c>
     </row>
     <row r="150">
@@ -7510,7 +7510,7 @@
         <v>8</v>
       </c>
       <c r="O150" t="n">
-        <v>0.2894654273986816</v>
+        <v>0.2923462390899658</v>
       </c>
     </row>
     <row r="151">
@@ -7557,7 +7557,7 @@
         <v>7</v>
       </c>
       <c r="O151" t="n">
-        <v>0.001271963119506836</v>
+        <v>0.002306938171386719</v>
       </c>
     </row>
     <row r="152">
@@ -7651,7 +7651,7 @@
         <v>7</v>
       </c>
       <c r="O153" t="n">
-        <v>0.0005590915679931641</v>
+        <v>0</v>
       </c>
     </row>
     <row r="154">
@@ -7933,7 +7933,7 @@
         <v>11</v>
       </c>
       <c r="O159" t="n">
-        <v>0.01398611068725586</v>
+        <v>0</v>
       </c>
     </row>
     <row r="160">
@@ -7980,7 +7980,7 @@
         <v>9</v>
       </c>
       <c r="O160" t="n">
-        <v>0.00110316276550293</v>
+        <v>0</v>
       </c>
     </row>
     <row r="161">
@@ -8027,7 +8027,7 @@
         <v>6</v>
       </c>
       <c r="O161" t="n">
-        <v>0.008305549621582031</v>
+        <v>0</v>
       </c>
     </row>
     <row r="162">
@@ -8168,7 +8168,7 @@
         <v>9</v>
       </c>
       <c r="O164" t="n">
-        <v>0.002242326736450195</v>
+        <v>0</v>
       </c>
     </row>
     <row r="165">
@@ -8215,7 +8215,7 @@
         <v>10</v>
       </c>
       <c r="O165" t="n">
-        <v>0</v>
+        <v>0.001004219055175781</v>
       </c>
     </row>
     <row r="166">
@@ -8262,7 +8262,7 @@
         <v>10</v>
       </c>
       <c r="O166" t="n">
-        <v>0</v>
+        <v>0.000919342041015625</v>
       </c>
     </row>
     <row r="167">
@@ -8450,7 +8450,7 @@
         <v>11</v>
       </c>
       <c r="O170" t="n">
-        <v>0</v>
+        <v>0.001102209091186523</v>
       </c>
     </row>
     <row r="171">
@@ -8544,7 +8544,7 @@
         <v>9</v>
       </c>
       <c r="O172" t="n">
-        <v>0.002647638320922852</v>
+        <v>0.008905172348022461</v>
       </c>
     </row>
     <row r="173">
@@ -8638,7 +8638,7 @@
         <v>9</v>
       </c>
       <c r="O174" t="n">
-        <v>0.00758051872253418</v>
+        <v>0</v>
       </c>
     </row>
     <row r="175">
@@ -8685,7 +8685,7 @@
         <v>3</v>
       </c>
       <c r="O175" t="n">
-        <v>0.001041889190673828</v>
+        <v>0</v>
       </c>
     </row>
     <row r="176">
@@ -8732,7 +8732,7 @@
         <v>3</v>
       </c>
       <c r="O176" t="n">
-        <v>0.01451730728149414</v>
+        <v>0.005504846572875977</v>
       </c>
     </row>
     <row r="177">

</xml_diff>